<commit_message>
chore: align richdata fixture rel URIs and fix formula-vba build
- Update linked-data-types richData fixture to use Excel-style Office 2017 relationship Type URIs in xl/_rels/metadata.xml.rels.

- Fix formula-vba compilation by importing DigestAlg in signature OID parsing helpers.

Test: cargo test -p formula-xlsx --test linked_data_types_fixture
</commit_message>
<xml_diff>
--- a/fixtures/xlsx/richdata/linked-data-types.xlsx
+++ b/fixtures/xlsx/richdata/linked-data-types.xlsx
@@ -36,6 +36,15 @@
       <rc t="1" v="1"/>
     </bk>
   </valueMetadata>
+  <!-- cm uses 1-based indexing, matching vm. -->
+  <cellMetadata count="2">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+  </cellMetadata>
 </metadata>
 </file>
 
@@ -126,14 +135,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr" vm="1">
+      <c r="A1" t="inlineStr" vm="1" cm="1">
         <is>
           <t>MSFT</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr" vm="2">
+      <c r="A2" t="inlineStr" vm="2" cm="2">
         <is>
           <t>Seattle</t>
         </is>

</xml_diff>